<commit_message>
fixed cape may naming error
</commit_message>
<xml_diff>
--- a/data/indicators.xlsx
+++ b/data/indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miahollie/data-projects/2024/projects/nj-voter-changes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E97F23A-D23E-E74F-B40A-E26142CF4FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA744E5-9B65-0B44-AA65-7D4EF5F9D2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19620" xr2:uid="{CB3E587A-8561-5B4C-81EF-55B0043C816A}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>camden</t>
   </si>
   <si>
-    <t>cape_may</t>
-  </si>
-  <si>
     <t>cumberland</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>county</t>
+  </si>
+  <si>
+    <t>cape may</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F47ECC-1B16-8542-95C4-089A29CE750B}">
   <dimension ref="A1:DB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BE1" sqref="BE1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,322 +825,322 @@
   <sheetData>
     <row r="1" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>42</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>55</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>57</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>58</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>59</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>60</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>61</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>62</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>63</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>65</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>66</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>67</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>68</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>69</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>70</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>71</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>72</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>73</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>74</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>75</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>76</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>77</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>78</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>79</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>80</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>81</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>82</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>83</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>84</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>85</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>86</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>87</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>89</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>90</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>91</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>92</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>93</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>94</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>95</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>96</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>97</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>98</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>99</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>100</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>101</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>102</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>103</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>104</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>105</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>106</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>107</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>108</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>109</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>110</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>111</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>112</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>113</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>114</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>115</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>116</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>117</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>118</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>119</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>120</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>121</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>122</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>123</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>124</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:106" x14ac:dyDescent="0.2">
@@ -2425,7 +2425,7 @@
     </row>
     <row r="6" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="B6" s="2">
         <v>14405</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="7" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>25684</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="8" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>209583</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="9" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>71782</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="10" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>173890</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="11" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>17712</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="12" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>83372</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="13" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>171985</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="14" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2">
         <v>107140</v>
@@ -5305,7 +5305,7 @@
     </row>
     <row r="15" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2">
         <v>70886</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="16" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2">
         <v>79872</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="17" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>82759</v>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="18" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2">
         <v>13629</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="19" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2">
         <v>50005</v>
@@ -6905,7 +6905,7 @@
     </row>
     <row r="20" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2">
         <v>16317</v>
@@ -7225,7 +7225,7 @@
     </row>
     <row r="21" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>124349</v>
@@ -7545,7 +7545,7 @@
     </row>
     <row r="22" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2">
         <v>14788</v>

</xml_diff>